<commit_message>
Second set of Arna's tests
</commit_message>
<xml_diff>
--- a/CRM/Arna Test scenarios/Test cases.xlsx
+++ b/CRM/Arna Test scenarios/Test cases.xlsx
@@ -25,8 +25,97 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sunjeet Khokhar</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sunjeet Khokhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1. repository items have meaningful names 
+2. no hard coding , use variables
+3. variables data bound where ever required
+4. no hard sleeps use "wait_for"
+5. validation based on unique element ids or unique element property ,wherever possible
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sunjeet Khokhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Are they tests being consumed and utilized by the business?
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sunjeet Khokhar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Are the tests integrated with a Continuous Integration engine, so that they can be batched to run automatically and/or on demand
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="117">
   <si>
     <t>Business Process</t>
   </si>
@@ -539,12 +628,15 @@
   <si>
     <t>Can_not_create_delete_account.rxrec</t>
   </si>
+  <si>
+    <t>account_details_edit_is_read_only.rxrec</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,6 +660,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1143,14 +1248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,8 +1265,8 @@
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="57.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -1545,6 +1650,12 @@
       <c r="D32" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="K32" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1911,6 +2022,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1921,7 +2033,7 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update DOD in test case list
</commit_message>
<xml_diff>
--- a/CRM/Arna Test scenarios/Test cases.xlsx
+++ b/CRM/Arna Test scenarios/Test cases.xlsx
@@ -105,7 +105,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Are the tests integrated with a Continuous Integration engine, so that they can be batched to run automatically and/or on demand
+Are the tests integrated with a Continuous Integration engine, so that they can be batched to run with out human intervention and/or on demand
 </t>
         </r>
       </text>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="118">
   <si>
     <t>Business Process</t>
   </si>
@@ -631,12 +631,15 @@
   <si>
     <t>account_details_edit_is_read_only.rxrec</t>
   </si>
+  <si>
+    <t>DEFINITION OF DONE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +677,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -909,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -969,6 +980,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1288,6 +1303,14 @@
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="14"/>
+      <c r="E2" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
@@ -1298,22 +1321,22 @@
       <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="32" t="s">
         <v>107</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -2020,6 +2043,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:J2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>